<commit_message>
Gráfico de Dispersão e PROCV
</commit_message>
<xml_diff>
--- a/Gráfico de Dispersão.xlsx
+++ b/Gráfico de Dispersão.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="199" documentId="11_92485C45C1F39E42E268565A893E8C18510380CC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DCDD0ECC-F4CE-410D-9638-C71AE2AFDA00}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Meu Drive\DISCIPLINAS\INFO BÁSICA\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C79C92C7-7379-450C-A70B-B61F3AFC8BEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Avaliação de Empresas" sheetId="1" r:id="rId1"/>
@@ -130,7 +135,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5902,9 +5907,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -5942,7 +5947,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -6048,7 +6053,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -6190,7 +6195,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -6201,17 +6206,17 @@
   <dimension ref="A3:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:C13"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -6222,7 +6227,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -6233,7 +6238,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -6244,7 +6249,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -6255,7 +6260,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -6266,7 +6271,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -6277,7 +6282,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -6288,7 +6293,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -6299,7 +6304,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -6310,7 +6315,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -6321,7 +6326,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -6346,15 +6351,15 @@
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" customWidth="1"/>
+    <col min="4" max="4" width="22.44140625" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" ht="45.75">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -6368,7 +6373,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="2:5">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -6382,7 +6387,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="2:5">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -6396,7 +6401,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="2:5">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -6410,7 +6415,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:5">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>6</v>
       </c>
@@ -6424,7 +6429,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="2:5">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>7</v>
       </c>
@@ -6438,7 +6443,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="2:5">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>8</v>
       </c>
@@ -6452,7 +6457,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="2:5">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>9</v>
       </c>
@@ -6466,7 +6471,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="2:5">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>10</v>
       </c>
@@ -6480,7 +6485,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="2:5">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>11</v>
       </c>
@@ -6494,7 +6499,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="2:5">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>12</v>
       </c>
@@ -6522,14 +6527,14 @@
       <selection activeCell="T23" sqref="T23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="15.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="2"/>
+    <col min="2" max="2" width="15.109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
@@ -6540,7 +6545,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
@@ -6551,7 +6556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
@@ -6562,7 +6567,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>19</v>
       </c>
@@ -6573,7 +6578,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>20</v>
       </c>
@@ -6584,7 +6589,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
@@ -6595,7 +6600,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
@@ -6606,7 +6611,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>23</v>
       </c>
@@ -6631,9 +6636,9 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -6668,7 +6673,7 @@
         <v>0.92339000000000004</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -6703,7 +6708,7 @@
         <v>0.89919000000000004</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -6738,7 +6743,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -6797,17 +6802,17 @@
       <selection activeCell="A3" sqref="A3:B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -6815,7 +6820,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>-10</v>
       </c>
@@ -6824,7 +6829,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>-9</v>
       </c>
@@ -6833,7 +6838,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>-8</v>
       </c>
@@ -6842,7 +6847,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>-7</v>
       </c>
@@ -6851,7 +6856,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>-6</v>
       </c>
@@ -6860,7 +6865,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>-5</v>
       </c>
@@ -6869,7 +6874,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>-4</v>
       </c>
@@ -6878,7 +6883,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>-3</v>
       </c>
@@ -6887,7 +6892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>-2</v>
       </c>
@@ -6896,7 +6901,7 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>-1</v>
       </c>
@@ -6905,7 +6910,7 @@
         <v>-8</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>0</v>
       </c>
@@ -6914,7 +6919,7 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>1</v>
       </c>
@@ -6923,7 +6928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2</v>
       </c>
@@ -6932,7 +6937,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>3</v>
       </c>
@@ -6941,7 +6946,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>4</v>
       </c>
@@ -6950,7 +6955,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>5</v>
       </c>
@@ -6959,7 +6964,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>6</v>
       </c>
@@ -6968,7 +6973,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>7</v>
       </c>
@@ -6977,7 +6982,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>8</v>
       </c>
@@ -6986,7 +6991,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>9</v>
       </c>
@@ -6995,7 +7000,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>10</v>
       </c>

</xml_diff>